<commit_message>
Final Doc Code Analysis - Review
</commit_message>
<xml_diff>
--- a/Team-Meeting-Info.xlsx
+++ b/Team-Meeting-Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konetisaipradeep/IdeaProjects/Softwareassurance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAF2C42-AFD0-0D47-AAF9-89AB7C81E4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB75835-8448-C344-AF78-FB718D2ADB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <r>
       <t xml:space="preserve">                                        </t>
@@ -263,6 +263,36 @@
   </si>
   <si>
     <t>Full</t>
+  </si>
+  <si>
+    <t>The team gathered to discuss more on code analysis, tools, and task segregation.</t>
+  </si>
+  <si>
+    <t>Discussion on manual and automated code analysis.</t>
+  </si>
+  <si>
+    <t>Team gathered to discuss more on the feedback received from team check-in with the professor</t>
+  </si>
+  <si>
+    <t>Set proper code review strategy and related CWE’s are consolidated for further analysis.</t>
+  </si>
+  <si>
+    <t>Team discussed on their respective manual and automated code analysis progress.</t>
+  </si>
+  <si>
+    <t>Peer review and refined some of the code review strategies for further analysis.</t>
+  </si>
+  <si>
+    <t>Other than all these meetings team was actively available on WhatsApp as it was a big assignment and discussed any blockage on the assigned tasks then and there.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7:30 to 9 PM</t>
+  </si>
+  <si>
+    <t>7:00 to 8:30 PM</t>
+  </si>
+  <si>
+    <t>12:00 to 1:00PM</t>
   </si>
 </sst>
 </file>
@@ -361,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -386,6 +416,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -606,14 +639,14 @@
   <dimension ref="A1:G1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A10" sqref="A10:D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="100.83203125" customWidth="1"/>
+    <col min="3" max="3" width="139.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="26" width="7.6640625" customWidth="1"/>
   </cols>
@@ -1177,24 +1210,132 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="13">
+        <v>44165</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="14"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="14"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="13">
+        <v>44166</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="14"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="14"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="13">
+        <v>44168</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="14"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="14"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="14"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="13">
+        <v>44170</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>